<commit_message>
Adding data in the given part of TestLoanAndTerm-WithDataInGivenSequence for SimpleBankLoan model
</commit_message>
<xml_diff>
--- a/Models/SimpleBankLoan/data.xlsx
+++ b/Models/SimpleBankLoan/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>loan</t>
   </si>
@@ -25,6 +25,9 @@
     <t>expected_result</t>
   </si>
   <si>
+    <t>obtained_result</t>
+  </si>
+  <si>
     <t>status</t>
   </si>
   <si>
@@ -32,9 +35,6 @@
   </si>
   <si>
     <t>Low-Volume Loan Long-Term</t>
-  </si>
-  <si>
-    <t>passed</t>
   </si>
 </sst>
 </file>
@@ -366,19 +366,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D2" sqref="D2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="3" max="3" width="27.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="28.90625" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,144 +392,117 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
-        <v>322</v>
+        <v>882</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
-        <v>762</v>
+        <v>928</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>138</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>824</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>244</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>638</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>290</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>184</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>140</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>109</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>877</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>298</v>
-      </c>
-      <c r="B8">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>581</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10">
-        <v>788</v>
+        <v>827</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>678</v>
+      </c>
+      <c r="B11">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>522</v>
-      </c>
-      <c r="B11">
-        <v>8</v>
-      </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>